<commit_message>
modif preparation nmix data
</commit_message>
<xml_diff>
--- a/3.results/model_selection/fou_de_bassan_HR_2_covariates_blocks.xlsx
+++ b/3.results/model_selection/fou_de_bassan_HR_2_covariates_blocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schroll\Documents\stage_M2\3.results\model_selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Documents\stage_M2\3.results\model_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1B1814-98BC-4AA0-B92C-46DF80023583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98156D0F-4911-4921-9AE8-58F32213C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="static_covs" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +353,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,11 +383,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="33">
     <dxf>
       <font>
         <b/>
@@ -461,90 +470,6 @@
         <color rgb="FFFFB6C1"/>
         <name val="Calibri"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -652,90 +577,6 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <sz val="11"/>
         <color rgb="FFFFB6C1"/>
@@ -813,90 +654,6 @@
         <color rgb="FFFFB6C1"/>
         <name val="Calibri"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1208,9 +965,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1044,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1356,7 +1113,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -1429,7 +1186,7 @@
       </c>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1502,7 +1259,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1580,55 +1337,16 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
-    <cfRule type="cellIs" dxfId="53" priority="28" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="cellIs" dxfId="52" priority="27" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F5">
-    <cfRule type="cellIs" dxfId="51" priority="26" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
-    <cfRule type="cellIs" dxfId="50" priority="25" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
-    <cfRule type="cellIs" dxfId="49" priority="24" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
-    <cfRule type="cellIs" dxfId="48" priority="23" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
-    <cfRule type="cellIs" dxfId="47" priority="22" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K5">
-    <cfRule type="cellIs" dxfId="46" priority="21" operator="between">
+  <conditionalFormatting sqref="D2:K5">
+    <cfRule type="cellIs" dxfId="32" priority="21" operator="between">
       <formula>0.1</formula>
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L5">
+    <cfRule type="expression" dxfId="31" priority="19">
+      <formula>L2&lt;357</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -1637,11 +1355,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="19">
-      <formula>L2&lt;357</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M5">
+    <cfRule type="expression" dxfId="30" priority="17">
+      <formula>M2&lt;540</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -1650,11 +1368,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="17">
-      <formula>M2&lt;540</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N5">
+    <cfRule type="expression" dxfId="29" priority="15">
+      <formula>N2&lt;190</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1663,11 +1381,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="15">
-      <formula>N2&lt;190</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O5">
+    <cfRule type="expression" dxfId="28" priority="13">
+      <formula>O2&lt;53</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1676,11 +1394,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="13">
-      <formula>O2&lt;53</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P5">
+    <cfRule type="expression" dxfId="27" priority="11">
+      <formula>P2&lt;1137</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1689,11 +1407,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="11">
-      <formula>P2&lt;1137</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5">
+    <cfRule type="expression" dxfId="26" priority="9">
+      <formula>Q2&lt;353</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1702,11 +1420,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="9">
-      <formula>Q2&lt;353</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R5">
+    <cfRule type="expression" dxfId="25" priority="7">
+      <formula>R2&lt;539</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1715,11 +1433,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="7">
-      <formula>R2&lt;539</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S5">
+    <cfRule type="expression" dxfId="24" priority="5">
+      <formula>S2&lt;193</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1728,11 +1446,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="5">
-      <formula>S2&lt;193</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T5">
+    <cfRule type="expression" dxfId="23" priority="3">
+      <formula>T2&lt;57</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1741,11 +1459,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="3">
-      <formula>T2&lt;57</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U5">
+    <cfRule type="expression" dxfId="22" priority="1">
+      <formula>U2&lt;1140</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1753,9 +1471,6 @@
         <color rgb="FFFF0000"/>
         <color rgb="FFFFFFFF"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="1">
-      <formula>U2&lt;1140</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1771,9 +1486,9 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1589,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1951,7 +1666,7 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2032,7 +1747,7 @@
       </c>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2113,7 +1828,7 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -2194,7 +1909,7 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -2275,7 +1990,7 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -2360,7 +2075,7 @@
       </c>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -2445,7 +2160,7 @@
       </c>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -2530,7 +2245,7 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -2615,7 +2330,7 @@
       </c>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2700,7 +2415,7 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -2785,7 +2500,7 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -2874,7 +2589,7 @@
       </c>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -2963,7 +2678,7 @@
       </c>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -3052,7 +2767,7 @@
       </c>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -3141,7 +2856,7 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -3234,7 +2949,7 @@
       </c>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -3315,7 +3030,7 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -3396,7 +3111,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -3482,55 +3197,16 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E20">
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F20">
-    <cfRule type="cellIs" dxfId="33" priority="26" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
-    <cfRule type="cellIs" dxfId="30" priority="23" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K20">
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="between">
+  <conditionalFormatting sqref="D2:K20">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="between">
       <formula>0.1</formula>
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L20">
+    <cfRule type="expression" dxfId="20" priority="19">
+      <formula>L2&lt;359</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3539,11 +3215,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="19">
-      <formula>L2&lt;359</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M20">
+    <cfRule type="expression" dxfId="19" priority="17">
+      <formula>M2&lt;556</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3552,11 +3228,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="17">
-      <formula>M2&lt;556</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N20">
+    <cfRule type="expression" dxfId="18" priority="15">
+      <formula>N2&lt;187</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3565,11 +3241,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="15">
-      <formula>N2&lt;187</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O20">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>O2&lt;51</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3578,11 +3254,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="13">
-      <formula>O2&lt;51</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P20">
+    <cfRule type="expression" dxfId="16" priority="11">
+      <formula>P2&lt;1150</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3591,11 +3267,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="11">
-      <formula>P2&lt;1150</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q20">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>Q2&lt;354</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3604,11 +3280,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="9">
-      <formula>Q2&lt;354</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R20">
+    <cfRule type="expression" dxfId="14" priority="7">
+      <formula>R2&lt;555</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3617,11 +3293,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
-      <formula>R2&lt;555</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S20">
+    <cfRule type="expression" dxfId="13" priority="5">
+      <formula>S2&lt;192</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3630,11 +3306,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="5">
-      <formula>S2&lt;192</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T20">
+    <cfRule type="expression" dxfId="12" priority="3">
+      <formula>T2&lt;56</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3643,11 +3319,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
-      <formula>T2&lt;56</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U20">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>U2&lt;1155</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3655,9 +3331,6 @@
         <color rgb="FFFF0000"/>
         <color rgb="FFFFFFFF"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="1">
-      <formula>U2&lt;1155</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3670,12 +3343,12 @@
   <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3770,7 +3443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -3845,7 +3518,7 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -3924,7 +3597,7 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -4003,7 +3676,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -4082,7 +3755,7 @@
       </c>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -4161,7 +3834,7 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4240,7 +3913,7 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -4323,7 +3996,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -4406,7 +4079,7 @@
       </c>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -4489,7 +4162,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -4572,7 +4245,7 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -4655,7 +4328,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -4738,7 +4411,7 @@
       </c>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -4821,7 +4494,7 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -4904,7 +4577,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -4987,8 +4660,8 @@
       </c>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B17" s="1">
@@ -5070,7 +4743,7 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
@@ -5157,7 +4830,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
@@ -5244,7 +4917,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -5331,7 +5004,7 @@
       </c>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -5418,7 +5091,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>88</v>
       </c>
@@ -5505,7 +5178,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -5592,7 +5265,7 @@
       </c>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>90</v>
       </c>
@@ -5679,7 +5352,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>91</v>
       </c>
@@ -5766,7 +5439,7 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>92</v>
       </c>
@@ -5853,7 +5526,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>93</v>
       </c>
@@ -5940,7 +5613,7 @@
       </c>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>94</v>
       </c>
@@ -6031,7 +5704,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>95</v>
       </c>
@@ -6122,7 +5795,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>96</v>
       </c>
@@ -6213,7 +5886,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>97</v>
       </c>
@@ -6304,7 +5977,7 @@
       </c>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>98</v>
       </c>
@@ -6395,7 +6068,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -6491,55 +6164,16 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F33">
-    <cfRule type="cellIs" dxfId="15" priority="26" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
-    <cfRule type="cellIs" dxfId="14" priority="25" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
-    <cfRule type="cellIs" dxfId="12" priority="23" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J33">
-    <cfRule type="cellIs" dxfId="11" priority="22" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K33">
+  <conditionalFormatting sqref="D2:K33">
     <cfRule type="cellIs" dxfId="10" priority="21" operator="between">
       <formula>0.1</formula>
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
+    <cfRule type="expression" dxfId="9" priority="19">
+      <formula>L2&lt;356</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -6548,11 +6182,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="19">
-      <formula>L2&lt;356</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M33">
+    <cfRule type="expression" dxfId="8" priority="17">
+      <formula>M2&lt;554</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -6561,11 +6195,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="17">
-      <formula>M2&lt;554</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N33">
+    <cfRule type="expression" dxfId="7" priority="15">
+      <formula>N2&lt;191</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -6574,11 +6208,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
-      <formula>N2&lt;191</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O33">
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>O2&lt;54</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -6587,11 +6221,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="13">
-      <formula>O2&lt;54</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P33">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>P2&lt;1155</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -6600,11 +6234,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11">
-      <formula>P2&lt;1155</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q33">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>Q2&lt;354</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -6613,11 +6247,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
-      <formula>Q2&lt;354</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R33">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>R2&lt;554</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -6626,11 +6260,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>R2&lt;554</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S33">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>S2&lt;193</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6639,11 +6273,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
-      <formula>S2&lt;193</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T33">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>T2&lt;58</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6652,11 +6286,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>T2&lt;58</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U33">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>U2&lt;1162</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6665,9 +6299,6 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>U2&lt;1162</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>